<commit_message>
&& - №71563216 от 11.10.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Austria/#EURO#Austria#Regular#[2002-present]#circulation_quality%varieties.xlsx
+++ b/Collections/EURO/Austria/#EURO#Austria#Regular#[2002-present]#circulation_quality%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Austria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E5C7DA-7FE2-4909-8BF0-7F5497B314C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBFFFB-FAC9-495D-BD94-FFEF23C60067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="33150" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1cent" sheetId="4" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F23">
+  <conditionalFormatting sqref="F23 F20">
     <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -2021,7 +2021,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F24">
+  <conditionalFormatting sqref="F24 F21">
     <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -2046,11 +2046,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B2"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2161,7 +2161,7 @@
         <v>156520000</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2593,7 +2593,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F23">
+  <conditionalFormatting sqref="F23 F20">
     <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -2625,7 +2625,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F24">
+  <conditionalFormatting sqref="F24 F21">
     <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -2650,7 +2650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3197,7 +3197,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F23">
+  <conditionalFormatting sqref="F23 F20">
     <cfRule type="containsText" dxfId="21" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -3229,7 +3229,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F24">
+  <conditionalFormatting sqref="F24 F21">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -3845,7 +3845,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F23">
+  <conditionalFormatting sqref="F23 F20">
     <cfRule type="containsText" dxfId="18" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -3877,7 +3877,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F24">
+  <conditionalFormatting sqref="F24 F21">
     <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -4493,7 +4493,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F23">
+  <conditionalFormatting sqref="F23 F20">
     <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -4525,7 +4525,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F24">
+  <conditionalFormatting sqref="F24 F21">
     <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -4545,7 +4545,7 @@
       <formula>NOT(ISERROR(SEARCH(("*-"),(F19))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19 F22">
+  <conditionalFormatting sqref="F22 F19">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -5158,7 +5158,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F23">
+  <conditionalFormatting sqref="F23 F20">
     <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -5190,7 +5190,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F24">
+  <conditionalFormatting sqref="F24 F21">
     <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -6456,7 +6456,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F20 F22 F24">
+  <conditionalFormatting sqref="F22 F20 F24">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -6488,7 +6488,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21 F23">
+  <conditionalFormatting sqref="F23 F21">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
&& - №78664079 от 22.05.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Austria/#EURO#Austria#Regular#[2002-present]#circulation_quality%varieties.xlsx
+++ b/Collections/EURO/Austria/#EURO#Austria#Regular#[2002-present]#circulation_quality%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Austria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBFFFB-FAC9-495D-BD94-FFEF23C60067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA116C6-9CE8-496F-89B5-EF9AD822425C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="33150" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1cent" sheetId="4" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F23 F20">
+  <conditionalFormatting sqref="F20 F23">
     <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -2021,7 +2021,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24 F21">
+  <conditionalFormatting sqref="F21 F24">
     <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -2046,11 +2046,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2593,7 +2593,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F23 F20">
+  <conditionalFormatting sqref="F20 F23">
     <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -2625,7 +2625,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24 F21">
+  <conditionalFormatting sqref="F21 F24">
     <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -2650,11 +2650,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3007,7 +3007,7 @@
         <v>61060000</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3197,7 +3197,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F23 F20">
+  <conditionalFormatting sqref="F20 F23">
     <cfRule type="containsText" dxfId="21" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -3229,7 +3229,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24 F21">
+  <conditionalFormatting sqref="F21 F24">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -3845,7 +3845,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="F23 F20">
+  <conditionalFormatting sqref="F20 F23">
     <cfRule type="containsText" dxfId="18" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -3877,7 +3877,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24 F21">
+  <conditionalFormatting sqref="F21 F24">
     <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -4493,7 +4493,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F23 F20">
+  <conditionalFormatting sqref="F20 F23">
     <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -4525,7 +4525,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24 F21">
+  <conditionalFormatting sqref="F21 F24">
     <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -4545,7 +4545,7 @@
       <formula>NOT(ISERROR(SEARCH(("*-"),(F19))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22 F19">
+  <conditionalFormatting sqref="F19 F22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -5158,7 +5158,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F23 F20">
+  <conditionalFormatting sqref="F20 F23">
     <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -5190,7 +5190,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24 F21">
+  <conditionalFormatting sqref="F21 F24">
     <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>
@@ -6456,7 +6456,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="F22 F20 F24">
+  <conditionalFormatting sqref="F20 F22 F24">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
     </cfRule>
@@ -6488,7 +6488,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23 F21">
+  <conditionalFormatting sqref="F21 F23">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
     </cfRule>

</xml_diff>